<commit_message>
config param to find the best for the model
</commit_message>
<xml_diff>
--- a/restaurant_analytics/predictions.xlsx
+++ b/restaurant_analytics/predictions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cardi\Documents\git-repo\swe_dev\restaurant_analytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D98B66-4DFF-44DC-9C1D-D02285D2379F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3E3DDA-07BD-43CF-8AA5-9B1C5306D96E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7515" yWindow="540" windowWidth="21600" windowHeight="11295" xr2:uid="{3707E157-C599-42C4-9FA7-BB38E1E45B47}"/>
+    <workbookView xWindow="4350" yWindow="2100" windowWidth="21600" windowHeight="11295" xr2:uid="{3707E157-C599-42C4-9FA7-BB38E1E45B47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -468,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97BA9C31-D39F-4D4C-A155-5360FBB6FAD9}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,77 +507,74 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="C2" s="4">
-        <v>45728</v>
+        <v>45730</v>
       </c>
       <c r="D2">
-        <v>55</v>
+        <v>130</v>
       </c>
       <c r="E2">
-        <v>43.9</v>
+        <v>58.5</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>8.1</v>
+        <v>12.6</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C3" s="4">
-        <v>45729</v>
-      </c>
-      <c r="D3">
-        <v>50</v>
+        <v>45731</v>
       </c>
       <c r="E3">
-        <v>49.6</v>
+        <v>54.1</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>7.5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="C4" s="4">
-        <v>45730</v>
+        <v>45732</v>
       </c>
       <c r="D4">
-        <v>137</v>
+        <v>55</v>
       </c>
       <c r="E4">
-        <v>58.5</v>
+        <v>40.5</v>
       </c>
       <c r="F4">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <v>12.6</v>
@@ -585,71 +582,71 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B5">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="C5" s="4">
-        <v>45731</v>
+        <v>45733</v>
       </c>
       <c r="D5">
-        <v>145</v>
+        <v>50</v>
       </c>
       <c r="E5">
-        <v>54.1</v>
+        <v>39.4</v>
       </c>
       <c r="F5">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
-        <v>18</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="C6" s="4">
-        <v>45732</v>
+        <v>45734</v>
       </c>
       <c r="D6">
         <v>55</v>
       </c>
       <c r="E6">
-        <v>40.5</v>
+        <v>42.3</v>
       </c>
       <c r="F6">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>12.6</v>
+        <v>11.1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B7">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="C7" s="4">
-        <v>45733</v>
+        <v>45735</v>
       </c>
       <c r="D7">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="E7">
-        <v>39.4</v>
+        <v>43.7</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -658,205 +655,159 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>10.5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B8">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C8" s="4">
-        <v>45734</v>
+        <v>45736</v>
       </c>
       <c r="D8">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="E8">
-        <v>42.3</v>
+        <v>44.8</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H8">
-        <v>11.1</v>
+        <v>11.2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B9">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="C9" s="4">
-        <v>45735</v>
+        <v>45737</v>
       </c>
       <c r="D9">
-        <v>60</v>
-      </c>
-      <c r="E9">
-        <v>43.7</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>11</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B10">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="C10" s="4">
-        <v>45736</v>
+        <v>45738</v>
       </c>
       <c r="D10">
-        <v>100</v>
-      </c>
-      <c r="E10">
-        <v>44.8</v>
-      </c>
-      <c r="F10">
-        <v>0.8</v>
-      </c>
-      <c r="G10">
-        <v>0.1</v>
-      </c>
-      <c r="H10">
-        <v>11.2</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B11">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="C11" s="4">
-        <v>45737</v>
+        <v>45739</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B12">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="C12" s="4">
-        <v>45738</v>
+        <v>45740</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B13">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="C13" s="4">
-        <v>45739</v>
+        <v>45741</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B14">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="C14" s="4">
-        <v>45740</v>
+        <v>45742</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B15">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="C15" s="4">
-        <v>45741</v>
+        <v>45743</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B16">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C16" s="4">
-        <v>45742</v>
+        <v>45744</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B17">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="C17" s="4">
-        <v>45743</v>
+        <v>45745</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B18">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="C18" s="4">
-        <v>45744</v>
+        <v>45746</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B19">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="C19" s="4">
-        <v>45745</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="B20">
-        <v>374</v>
-      </c>
-      <c r="C20" s="4">
-        <v>45746</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>2</v>
-      </c>
-      <c r="B21">
-        <v>375</v>
-      </c>
-      <c r="C21" s="4">
         <v>45747</v>
       </c>
     </row>

</xml_diff>